<commit_message>
Update for the new mag types. Updated data files as well.
</commit_message>
<xml_diff>
--- a/data/Magnet_PS_circuits.xlsx
+++ b/data/Magnet_PS_circuits.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t xml:space="preserve">Magnets per circuits per half-achromat</t>
   </si>
@@ -71,6 +71,15 @@
     <t xml:space="preserve">i01</t>
   </si>
   <si>
+    <t xml:space="preserve">j01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">k01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l01</t>
+  </si>
+  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
@@ -143,7 +152,16 @@
     <t xml:space="preserve">S1_comb</t>
   </si>
   <si>
+    <t xml:space="preserve">S2_comb</t>
+  </si>
+  <si>
     <t xml:space="preserve">S3_comb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S4_comb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S5_comb</t>
   </si>
   <si>
     <t xml:space="preserve">S6_comb</t>
@@ -247,15 +265,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,10 +538,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:P31"/>
+  <dimension ref="B2:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S33" activeCellId="0" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -597,10 +615,19 @@
       <c r="P4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="Q4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
@@ -642,12 +669,21 @@
         <v>1</v>
       </c>
       <c r="P5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2.5</v>
@@ -691,10 +727,19 @@
       <c r="P6" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="Q6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>0</v>
@@ -738,10 +783,19 @@
       <c r="P7" s="1" t="n">
         <v>0.5</v>
       </c>
+      <c r="Q7" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>1</v>
@@ -783,12 +837,21 @@
         <v>1</v>
       </c>
       <c r="P8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>1</v>
@@ -830,12 +893,21 @@
         <v>1</v>
       </c>
       <c r="P9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>2</v>
@@ -878,11 +950,20 @@
       </c>
       <c r="P10" s="1" t="n">
         <v>2</v>
+      </c>
+      <c r="Q10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>4</v>
@@ -926,10 +1007,19 @@
       <c r="P11" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="Q11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>0</v>
@@ -971,12 +1061,21 @@
         <v>0</v>
       </c>
       <c r="P12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>0</v>
@@ -1018,12 +1117,21 @@
         <v>0</v>
       </c>
       <c r="P13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>0</v>
@@ -1067,10 +1175,19 @@
       <c r="P14" s="1" t="n">
         <v>2</v>
       </c>
+      <c r="Q14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>0</v>
@@ -1114,10 +1231,19 @@
       <c r="P15" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>0</v>
@@ -1161,10 +1287,19 @@
       <c r="P16" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>1</v>
@@ -1206,12 +1341,21 @@
         <v>0</v>
       </c>
       <c r="P17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
@@ -1255,10 +1399,19 @@
       <c r="P18" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="Q18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>5</v>
@@ -1302,10 +1455,19 @@
       <c r="P19" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>1</v>
@@ -1348,11 +1510,20 @@
       </c>
       <c r="P20" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>1</v>
@@ -1395,11 +1566,20 @@
       </c>
       <c r="P21" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>0</v>
@@ -1441,12 +1621,21 @@
         <v>0</v>
       </c>
       <c r="P22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>1</v>
@@ -1488,12 +1677,21 @@
         <v>1</v>
       </c>
       <c r="P23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>1</v>
@@ -1535,12 +1733,21 @@
         <v>1</v>
       </c>
       <c r="P24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>1</v>
@@ -1582,12 +1789,21 @@
         <v>1</v>
       </c>
       <c r="P25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="S25" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>0</v>
@@ -1631,10 +1847,19 @@
       <c r="P26" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="Q26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>0</v>
@@ -1676,12 +1901,21 @@
         <v>0</v>
       </c>
       <c r="P27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" s="1" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>0</v>
@@ -1723,12 +1957,21 @@
         <v>1</v>
       </c>
       <c r="P28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>0</v>
@@ -1758,24 +2001,33 @@
         <v>0</v>
       </c>
       <c r="L29" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="M29" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="N29" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="P29" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>0</v>
@@ -1805,79 +2057,268 @@
         <v>0</v>
       </c>
       <c r="L30" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M30" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N30" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O30" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P30" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="2" t="n">
-        <f aca="false">SUM(C5:C30)</f>
+        <v>4</v>
+      </c>
+      <c r="Q30" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="R30" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="S32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="P33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <f aca="false">SUM(C5:C33)</f>
         <v>23.5</v>
       </c>
-      <c r="D31" s="2" t="n">
-        <f aca="false">SUM(D5:D30)</f>
+      <c r="D34" s="2" t="n">
+        <f aca="false">SUM(D5:D33)</f>
         <v>23.5</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <f aca="false">SUM(E5:E30)</f>
+      <c r="E34" s="2" t="n">
+        <f aca="false">SUM(E5:E33)</f>
         <v>23.5</v>
       </c>
-      <c r="F31" s="2" t="n">
-        <f aca="false">SUM(F5:F30)</f>
+      <c r="F34" s="2" t="n">
+        <f aca="false">SUM(F5:F33)</f>
         <v>23.5</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <f aca="false">SUM(G5:G30)</f>
+      <c r="G34" s="2" t="n">
+        <f aca="false">SUM(G5:G33)</f>
         <v>23.5</v>
       </c>
-      <c r="H31" s="2" t="n">
-        <f aca="false">SUM(H5:H30)</f>
+      <c r="H34" s="2" t="n">
+        <f aca="false">SUM(H5:H33)</f>
         <v>23.5</v>
       </c>
-      <c r="I31" s="2" t="n">
-        <f aca="false">SUM(I5:I30)</f>
+      <c r="I34" s="2" t="n">
+        <f aca="false">SUM(I5:I33)</f>
         <v>28.5</v>
       </c>
-      <c r="J31" s="2" t="n">
-        <f aca="false">SUM(J5:J30)</f>
+      <c r="J34" s="2" t="n">
+        <f aca="false">SUM(J5:J33)</f>
         <v>28.5</v>
       </c>
-      <c r="K31" s="2" t="n">
-        <f aca="false">SUM(K5:K30)</f>
+      <c r="K34" s="2" t="n">
+        <f aca="false">SUM(K5:K33)</f>
         <v>23.5</v>
       </c>
-      <c r="L31" s="2" t="n">
-        <f aca="false">SUM(L5:L30)</f>
+      <c r="L34" s="2" t="n">
+        <f aca="false">SUM(L5:L33)</f>
         <v>23.5</v>
       </c>
-      <c r="M31" s="2" t="n">
-        <f aca="false">SUM(M5:M30)</f>
+      <c r="M34" s="2" t="n">
+        <f aca="false">SUM(M5:M33)</f>
         <v>23.5</v>
       </c>
-      <c r="N31" s="2" t="n">
-        <f aca="false">SUM(N5:N30)</f>
+      <c r="N34" s="2" t="n">
+        <f aca="false">SUM(N5:N33)</f>
         <v>23.5</v>
       </c>
-      <c r="O31" s="2" t="n">
-        <f aca="false">SUM(O5:O30)</f>
+      <c r="O34" s="2" t="n">
+        <f aca="false">SUM(O5:O33)</f>
         <v>23.5</v>
       </c>
-      <c r="P31" s="2" t="n">
-        <f aca="false">SUM(P5:P30)</f>
+      <c r="P34" s="2" t="n">
+        <f aca="false">SUM(P5:P33)</f>
+        <v>23.5</v>
+      </c>
+      <c r="Q34" s="2" t="n">
+        <f aca="false">SUM(Q5:Q33)</f>
+        <v>23.5</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <f aca="false">SUM(R5:R33)</f>
+        <v>23.5</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <f aca="false">SUM(S5:S33)</f>
         <v>23.5</v>
       </c>
     </row>
@@ -1885,7 +2326,7 @@
   <mergeCells count="1">
     <mergeCell ref="C3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:P30">
+  <conditionalFormatting sqref="C5:S33">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>0</formula>
     </cfRule>
@@ -1905,23 +2346,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:Q31"/>
+  <dimension ref="B2:T34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q4" activeCellId="0" sqref="Q4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R32" activeCellId="0" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="17" style="0" width="6.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="6.9"/>
   </cols>
   <sheetData>
     <row r="2" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1936,6 +2378,9 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
@@ -1984,12 +2429,21 @@
         <v>15</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1" t="n">
         <f aca="false">RawData!C5*2</f>
@@ -2047,13 +2501,25 @@
         <f aca="false">RawData!P5*2</f>
         <v>2</v>
       </c>
-      <c r="Q5" s="1" t="s">
-        <v>45</v>
+      <c r="Q5" s="1" t="n">
+        <f aca="false">RawData!Q5*2</f>
+        <v>2</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <f aca="false">RawData!R5*2</f>
+        <v>2</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <f aca="false">RawData!S5*2</f>
+        <v>2</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="n">
         <f aca="false">RawData!C6*2</f>
@@ -2111,13 +2577,25 @@
         <f aca="false">RawData!P6*2</f>
         <v>4</v>
       </c>
-      <c r="Q6" s="1" t="s">
-        <v>45</v>
+      <c r="Q6" s="1" t="n">
+        <f aca="false">RawData!Q6*2</f>
+        <v>4</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <f aca="false">RawData!R6*2</f>
+        <v>4</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <f aca="false">RawData!S6*2</f>
+        <v>4</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C7" s="1" t="n">
         <f aca="false">RawData!C7*2</f>
@@ -2175,13 +2653,25 @@
         <f aca="false">RawData!P7*2</f>
         <v>1</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>45</v>
+      <c r="Q7" s="1" t="n">
+        <f aca="false">RawData!Q7*2</f>
+        <v>1</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <f aca="false">RawData!R7*2</f>
+        <v>1</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <f aca="false">RawData!S7*2</f>
+        <v>1</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="n">
         <f aca="false">RawData!C8*2</f>
@@ -2239,10 +2729,22 @@
         <f aca="false">RawData!P8*2</f>
         <v>2</v>
       </c>
+      <c r="Q8" s="1" t="n">
+        <f aca="false">RawData!Q8*2</f>
+        <v>2</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <f aca="false">RawData!R8*2</f>
+        <v>2</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <f aca="false">RawData!S8*2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="n">
         <f aca="false">RawData!C9*2</f>
@@ -2300,10 +2802,22 @@
         <f aca="false">RawData!P9*2</f>
         <v>2</v>
       </c>
+      <c r="Q9" s="1" t="n">
+        <f aca="false">RawData!Q9*2</f>
+        <v>2</v>
+      </c>
+      <c r="R9" s="1" t="n">
+        <f aca="false">RawData!R9*2</f>
+        <v>2</v>
+      </c>
+      <c r="S9" s="1" t="n">
+        <f aca="false">RawData!S9*2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1" t="n">
         <f aca="false">RawData!C10*2</f>
@@ -2361,10 +2875,22 @@
         <f aca="false">RawData!P10*2</f>
         <v>4</v>
       </c>
+      <c r="Q10" s="1" t="n">
+        <f aca="false">RawData!Q10*2</f>
+        <v>4</v>
+      </c>
+      <c r="R10" s="1" t="n">
+        <f aca="false">RawData!R10*2</f>
+        <v>2</v>
+      </c>
+      <c r="S10" s="1" t="n">
+        <f aca="false">RawData!S10*2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="n">
         <f aca="false">RawData!C11*2</f>
@@ -2422,10 +2948,22 @@
         <f aca="false">RawData!P11*2</f>
         <v>4</v>
       </c>
+      <c r="Q11" s="1" t="n">
+        <f aca="false">RawData!Q11*2</f>
+        <v>4</v>
+      </c>
+      <c r="R11" s="1" t="n">
+        <f aca="false">RawData!R11*2</f>
+        <v>0</v>
+      </c>
+      <c r="S11" s="1" t="n">
+        <f aca="false">RawData!S11*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
         <f aca="false">RawData!C12*2</f>
@@ -2483,10 +3021,22 @@
         <f aca="false">RawData!P12*2</f>
         <v>0</v>
       </c>
+      <c r="Q12" s="1" t="n">
+        <f aca="false">RawData!Q12*2</f>
+        <v>0</v>
+      </c>
+      <c r="R12" s="1" t="n">
+        <f aca="false">RawData!R12*2</f>
+        <v>0</v>
+      </c>
+      <c r="S12" s="1" t="n">
+        <f aca="false">RawData!S12*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="n">
         <f aca="false">RawData!C13*2</f>
@@ -2544,10 +3094,22 @@
         <f aca="false">RawData!P13*2</f>
         <v>0</v>
       </c>
+      <c r="Q13" s="1" t="n">
+        <f aca="false">RawData!Q13*2</f>
+        <v>0</v>
+      </c>
+      <c r="R13" s="1" t="n">
+        <f aca="false">RawData!R13*2</f>
+        <v>0</v>
+      </c>
+      <c r="S13" s="1" t="n">
+        <f aca="false">RawData!S13*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="n">
         <f aca="false">RawData!C14*2</f>
@@ -2605,10 +3167,22 @@
         <f aca="false">RawData!P14*2</f>
         <v>4</v>
       </c>
+      <c r="Q14" s="1" t="n">
+        <f aca="false">RawData!Q14*2</f>
+        <v>4</v>
+      </c>
+      <c r="R14" s="1" t="n">
+        <f aca="false">RawData!R14*2</f>
+        <v>4</v>
+      </c>
+      <c r="S14" s="1" t="n">
+        <f aca="false">RawData!S14*2</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="n">
         <f aca="false">RawData!C15*2</f>
@@ -2666,10 +3240,22 @@
         <f aca="false">RawData!P15*2</f>
         <v>0</v>
       </c>
+      <c r="Q15" s="1" t="n">
+        <f aca="false">RawData!Q15*2</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <f aca="false">RawData!R15*2</f>
+        <v>6</v>
+      </c>
+      <c r="S15" s="1" t="n">
+        <f aca="false">RawData!S15*2</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="n">
         <f aca="false">RawData!C16*2</f>
@@ -2727,10 +3313,22 @@
         <f aca="false">RawData!P16*2</f>
         <v>0</v>
       </c>
+      <c r="Q16" s="1" t="n">
+        <f aca="false">RawData!Q16*2</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="1" t="n">
+        <f aca="false">RawData!R16*2</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="1" t="n">
+        <f aca="false">RawData!S16*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1" t="n">
         <f aca="false">RawData!C17*2</f>
@@ -2788,10 +3386,22 @@
         <f aca="false">RawData!P17*2</f>
         <v>0</v>
       </c>
+      <c r="Q17" s="1" t="n">
+        <f aca="false">RawData!Q17*2</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="1" t="n">
+        <f aca="false">RawData!R17*2</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="1" t="n">
+        <f aca="false">RawData!S17*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C18" s="1" t="n">
         <f aca="false">RawData!C18*2</f>
@@ -2849,10 +3459,22 @@
         <f aca="false">RawData!P18*2</f>
         <v>2</v>
       </c>
+      <c r="Q18" s="1" t="n">
+        <f aca="false">RawData!Q18*2</f>
+        <v>2</v>
+      </c>
+      <c r="R18" s="1" t="n">
+        <f aca="false">RawData!R18*2</f>
+        <v>2</v>
+      </c>
+      <c r="S18" s="1" t="n">
+        <f aca="false">RawData!S18*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C19" s="1" t="n">
         <f aca="false">RawData!C19*2</f>
@@ -2910,10 +3532,22 @@
         <f aca="false">RawData!P19*2</f>
         <v>0</v>
       </c>
+      <c r="Q19" s="1" t="n">
+        <f aca="false">RawData!Q19*2</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="1" t="n">
+        <f aca="false">RawData!R19*2</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="1" t="n">
+        <f aca="false">RawData!S19*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="n">
         <f aca="false">RawData!C20*2</f>
@@ -2971,10 +3605,22 @@
         <f aca="false">RawData!P20*2</f>
         <v>2</v>
       </c>
+      <c r="Q20" s="1" t="n">
+        <f aca="false">RawData!Q20*2</f>
+        <v>2</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <f aca="false">RawData!R20*2</f>
+        <v>2</v>
+      </c>
+      <c r="S20" s="1" t="n">
+        <f aca="false">RawData!S20*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="n">
         <f aca="false">RawData!C21*2</f>
@@ -3032,10 +3678,22 @@
         <f aca="false">RawData!P21*2</f>
         <v>2</v>
       </c>
+      <c r="Q21" s="1" t="n">
+        <f aca="false">RawData!Q21*2</f>
+        <v>2</v>
+      </c>
+      <c r="R21" s="1" t="n">
+        <f aca="false">RawData!R21*2</f>
+        <v>0</v>
+      </c>
+      <c r="S21" s="1" t="n">
+        <f aca="false">RawData!S21*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C22" s="1" t="n">
         <f aca="false">RawData!C22*2</f>
@@ -3093,10 +3751,22 @@
         <f aca="false">RawData!P22*2</f>
         <v>0</v>
       </c>
+      <c r="Q22" s="1" t="n">
+        <f aca="false">RawData!Q22*2</f>
+        <v>0</v>
+      </c>
+      <c r="R22" s="1" t="n">
+        <f aca="false">RawData!R22*2</f>
+        <v>2</v>
+      </c>
+      <c r="S22" s="1" t="n">
+        <f aca="false">RawData!S22*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C23" s="1" t="n">
         <f aca="false">RawData!C23*2</f>
@@ -3154,13 +3824,25 @@
         <f aca="false">RawData!P23*2</f>
         <v>2</v>
       </c>
-      <c r="Q23" s="1" t="s">
-        <v>45</v>
+      <c r="Q23" s="1" t="n">
+        <f aca="false">RawData!Q23*2</f>
+        <v>2</v>
+      </c>
+      <c r="R23" s="1" t="n">
+        <f aca="false">RawData!R23*2</f>
+        <v>2</v>
+      </c>
+      <c r="S23" s="1" t="n">
+        <f aca="false">RawData!S23*2</f>
+        <v>2</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C24" s="1" t="n">
         <f aca="false">RawData!C24*2</f>
@@ -3218,13 +3900,25 @@
         <f aca="false">RawData!P24*2</f>
         <v>2</v>
       </c>
-      <c r="Q24" s="1" t="s">
-        <v>45</v>
+      <c r="Q24" s="1" t="n">
+        <f aca="false">RawData!Q24*2</f>
+        <v>2</v>
+      </c>
+      <c r="R24" s="1" t="n">
+        <f aca="false">RawData!R24*2</f>
+        <v>2</v>
+      </c>
+      <c r="S24" s="1" t="n">
+        <f aca="false">RawData!S24*2</f>
+        <v>2</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1" t="n">
         <f aca="false">RawData!C25*2</f>
@@ -3282,13 +3976,25 @@
         <f aca="false">RawData!P25*2</f>
         <v>2</v>
       </c>
-      <c r="Q25" s="1" t="s">
-        <v>45</v>
+      <c r="Q25" s="1" t="n">
+        <f aca="false">RawData!Q25*2</f>
+        <v>2</v>
+      </c>
+      <c r="R25" s="1" t="n">
+        <f aca="false">RawData!R25*2</f>
+        <v>2</v>
+      </c>
+      <c r="S25" s="1" t="n">
+        <f aca="false">RawData!S25*2</f>
+        <v>2</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C26" s="1" t="n">
         <f aca="false">RawData!C26*2</f>
@@ -3346,10 +4052,22 @@
         <f aca="false">RawData!P26*2</f>
         <v>0</v>
       </c>
+      <c r="Q26" s="1" t="n">
+        <f aca="false">RawData!Q26*2</f>
+        <v>0</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <f aca="false">RawData!R26*2</f>
+        <v>0</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <f aca="false">RawData!S26*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C27" s="1" t="n">
         <f aca="false">RawData!C27*2</f>
@@ -3407,10 +4125,22 @@
         <f aca="false">RawData!P27*2</f>
         <v>0</v>
       </c>
+      <c r="Q27" s="1" t="n">
+        <f aca="false">RawData!Q27*2</f>
+        <v>0</v>
+      </c>
+      <c r="R27" s="1" t="n">
+        <f aca="false">RawData!R27*2</f>
+        <v>0</v>
+      </c>
+      <c r="S27" s="1" t="n">
+        <f aca="false">RawData!S27*2</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1" t="n">
         <f aca="false">RawData!C28*2</f>
@@ -3468,10 +4198,22 @@
         <f aca="false">RawData!P28*2</f>
         <v>2</v>
       </c>
+      <c r="Q28" s="1" t="n">
+        <f aca="false">RawData!Q28*2</f>
+        <v>2</v>
+      </c>
+      <c r="R28" s="1" t="n">
+        <f aca="false">RawData!R28*2</f>
+        <v>4</v>
+      </c>
+      <c r="S28" s="1" t="n">
+        <f aca="false">RawData!S28*2</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C29" s="1" t="n">
         <f aca="false">RawData!C29*2</f>
@@ -3511,28 +4253,40 @@
       </c>
       <c r="L29" s="1" t="n">
         <f aca="false">RawData!L29*2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M29" s="1" t="n">
         <f aca="false">RawData!M29*2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N29" s="1" t="n">
         <f aca="false">RawData!N29*2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O29" s="1" t="n">
         <f aca="false">RawData!O29*2</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P29" s="1" t="n">
         <f aca="false">RawData!P29*2</f>
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1" t="n">
+        <f aca="false">RawData!Q29*2</f>
+        <v>0</v>
+      </c>
+      <c r="R29" s="1" t="n">
+        <f aca="false">RawData!R29*2</f>
+        <v>0</v>
+      </c>
+      <c r="S29" s="1" t="n">
+        <f aca="false">RawData!S29*2</f>
+        <v>2</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C30" s="1" t="n">
         <f aca="false">RawData!C30*2</f>
@@ -3572,83 +4326,326 @@
       </c>
       <c r="L30" s="1" t="n">
         <f aca="false">RawData!L30*2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M30" s="1" t="n">
         <f aca="false">RawData!M30*2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N30" s="1" t="n">
         <f aca="false">RawData!N30*2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O30" s="1" t="n">
         <f aca="false">RawData!O30*2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P30" s="1" t="n">
         <f aca="false">RawData!P30*2</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="2" t="n">
-        <f aca="false">SUM(C5:C30)</f>
+        <v>8</v>
+      </c>
+      <c r="Q30" s="1" t="n">
+        <f aca="false">RawData!Q30*2</f>
+        <v>8</v>
+      </c>
+      <c r="R30" s="1" t="n">
+        <f aca="false">RawData!R30*2</f>
+        <v>4</v>
+      </c>
+      <c r="S30" s="1" t="n">
+        <f aca="false">RawData!S30*2</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="false">RawData!C31*2</f>
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">RawData!D31*2</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="1" t="n">
+        <f aca="false">RawData!E31*2</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <f aca="false">RawData!F31*2</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <f aca="false">RawData!G31*2</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <f aca="false">RawData!H31*2</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <f aca="false">RawData!I31*2</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="1" t="n">
+        <f aca="false">RawData!J31*2</f>
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="n">
+        <f aca="false">RawData!K31*2</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <f aca="false">RawData!L31*2</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <f aca="false">RawData!M31*2</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="1" t="n">
+        <f aca="false">RawData!N31*2</f>
+        <v>0</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <f aca="false">RawData!O31*2</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <f aca="false">RawData!P31*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="1" t="n">
+        <f aca="false">RawData!Q31*2</f>
+        <v>0</v>
+      </c>
+      <c r="R31" s="1" t="n">
+        <f aca="false">RawData!R31*2</f>
+        <v>0</v>
+      </c>
+      <c r="S31" s="1" t="n">
+        <f aca="false">RawData!S31*2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <f aca="false">RawData!C32*2</f>
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">RawData!D32*2</f>
+        <v>0</v>
+      </c>
+      <c r="E32" s="1" t="n">
+        <f aca="false">RawData!E32*2</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <f aca="false">RawData!F32*2</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <f aca="false">RawData!G32*2</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <f aca="false">RawData!H32*2</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <f aca="false">RawData!I32*2</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="1" t="n">
+        <f aca="false">RawData!J32*2</f>
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="n">
+        <f aca="false">RawData!K32*2</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <f aca="false">RawData!L32*2</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <f aca="false">RawData!M32*2</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="1" t="n">
+        <f aca="false">RawData!N32*2</f>
+        <v>0</v>
+      </c>
+      <c r="O32" s="1" t="n">
+        <f aca="false">RawData!O32*2</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="1" t="n">
+        <f aca="false">RawData!P32*2</f>
+        <v>0</v>
+      </c>
+      <c r="Q32" s="1" t="n">
+        <f aca="false">RawData!Q32*2</f>
+        <v>0</v>
+      </c>
+      <c r="R32" s="1" t="n">
+        <f aca="false">RawData!R32*2</f>
+        <v>4</v>
+      </c>
+      <c r="S32" s="1" t="n">
+        <f aca="false">RawData!S32*2</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="2" t="n">
-        <f aca="false">SUM(D5:D30)</f>
+      <c r="C33" s="1" t="n">
+        <f aca="false">RawData!C33*2</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="false">RawData!D33*2</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="1" t="n">
+        <f aca="false">RawData!E33*2</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="1" t="n">
+        <f aca="false">RawData!F33*2</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <f aca="false">RawData!G33*2</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <f aca="false">RawData!H33*2</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <f aca="false">RawData!I33*2</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="1" t="n">
+        <f aca="false">RawData!J33*2</f>
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="n">
+        <f aca="false">RawData!K33*2</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <f aca="false">RawData!L33*2</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="1" t="n">
+        <f aca="false">RawData!M33*2</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="1" t="n">
+        <f aca="false">RawData!N33*2</f>
+        <v>0</v>
+      </c>
+      <c r="O33" s="1" t="n">
+        <f aca="false">RawData!O33*2</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="1" t="n">
+        <f aca="false">RawData!P33*2</f>
+        <v>2</v>
+      </c>
+      <c r="Q33" s="1" t="n">
+        <f aca="false">RawData!Q33*2</f>
+        <v>2</v>
+      </c>
+      <c r="R33" s="1" t="n">
+        <f aca="false">RawData!R33*2</f>
+        <v>0</v>
+      </c>
+      <c r="S33" s="1" t="n">
+        <f aca="false">RawData!S33*2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="2" t="n">
+        <f aca="false">SUM(C5:C33)</f>
         <v>47</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <f aca="false">SUM(E5:E30)</f>
+      <c r="D34" s="2" t="n">
+        <f aca="false">SUM(D5:D33)</f>
         <v>47</v>
       </c>
-      <c r="F31" s="2" t="n">
-        <f aca="false">SUM(F5:F30)</f>
+      <c r="E34" s="2" t="n">
+        <f aca="false">SUM(E5:E33)</f>
         <v>47</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <f aca="false">SUM(G5:G30)</f>
+      <c r="F34" s="2" t="n">
+        <f aca="false">SUM(F5:F33)</f>
         <v>47</v>
       </c>
-      <c r="H31" s="2" t="n">
-        <f aca="false">SUM(H5:H30)</f>
+      <c r="G34" s="2" t="n">
+        <f aca="false">SUM(G5:G33)</f>
         <v>47</v>
       </c>
-      <c r="I31" s="2" t="n">
-        <f aca="false">SUM(I5:I30)</f>
+      <c r="H34" s="2" t="n">
+        <f aca="false">SUM(H5:H33)</f>
+        <v>47</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <f aca="false">SUM(I5:I33)</f>
         <v>57</v>
       </c>
-      <c r="J31" s="2" t="n">
-        <f aca="false">SUM(J5:J30)</f>
+      <c r="J34" s="2" t="n">
+        <f aca="false">SUM(J5:J33)</f>
         <v>57</v>
       </c>
-      <c r="K31" s="2" t="n">
-        <f aca="false">SUM(K5:K30)</f>
+      <c r="K34" s="2" t="n">
+        <f aca="false">SUM(K5:K33)</f>
         <v>47</v>
       </c>
-      <c r="L31" s="2" t="n">
-        <f aca="false">SUM(L5:L30)</f>
+      <c r="L34" s="2" t="n">
+        <f aca="false">SUM(L5:L33)</f>
         <v>47</v>
       </c>
-      <c r="M31" s="2" t="n">
-        <f aca="false">SUM(M5:M30)</f>
+      <c r="M34" s="2" t="n">
+        <f aca="false">SUM(M5:M33)</f>
         <v>47</v>
       </c>
-      <c r="N31" s="2" t="n">
-        <f aca="false">SUM(N5:N30)</f>
+      <c r="N34" s="2" t="n">
+        <f aca="false">SUM(N5:N33)</f>
         <v>47</v>
       </c>
-      <c r="O31" s="2" t="n">
-        <f aca="false">SUM(O5:O30)</f>
+      <c r="O34" s="2" t="n">
+        <f aca="false">SUM(O5:O33)</f>
         <v>47</v>
       </c>
-      <c r="P31" s="2" t="n">
-        <f aca="false">SUM(P5:P30)</f>
+      <c r="P34" s="2" t="n">
+        <f aca="false">SUM(P5:P33)</f>
+        <v>47</v>
+      </c>
+      <c r="Q34" s="2" t="n">
+        <f aca="false">SUM(Q5:Q33)</f>
+        <v>47</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <f aca="false">SUM(R5:R33)</f>
+        <v>47</v>
+      </c>
+      <c r="S34" s="2" t="n">
+        <f aca="false">SUM(S5:S33)</f>
         <v>47</v>
       </c>
     </row>
@@ -3656,8 +4653,13 @@
   <mergeCells count="1">
     <mergeCell ref="C3:P3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C5:P30">
+  <conditionalFormatting sqref="C5:O33 Q5:S28 P29:S33">
     <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P5:P33">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>